<commit_message>
fix issue if the column value is empty
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -561,6 +561,9 @@
     <x:t>（汇总提炼上述“相对规范”）</x:t>
   </x:si>
   <x:si>
+    <x:t/>
+  </x:si>
+  <x:si>
     <x:t>监测评价机构盖章：                  法人签名：                  经办人签名：                        联系电话：</x:t>
   </x:si>
   <x:si>
@@ -571,9 +574,6 @@
   </x:si>
   <x:si>
     <x:t>单位2</x:t>
-  </x:si>
-  <x:si>
-    <x:t/>
   </x:si>
   <x:si>
     <x:t>该组织为一般性社团，会员总数未达到规定要求，仅有个人会员*个，单位会员*个。（会员数不能少于50）</x:t>
@@ -1432,19 +1432,22 @@
       <x:c r="CA2" s="0" t="s">
         <x:v>158</x:v>
       </x:c>
+      <x:c r="CB2" s="0" t="s">
+        <x:v>159</x:v>
+      </x:c>
       <x:c r="CC2" s="0" t="s">
-        <x:v>159</x:v>
+        <x:v>160</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:81">
       <x:c r="A3" s="0" t="s">
-        <x:v>160</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>161</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>162</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
         <x:v>84</x:v>
@@ -1459,13 +1462,13 @@
         <x:v>87</x:v>
       </x:c>
       <x:c r="H3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="I3" s="0" t="s">
         <x:v>164</x:v>
       </x:c>
       <x:c r="J3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="K3" s="0" t="s">
         <x:v>165</x:v>
@@ -1474,28 +1477,28 @@
         <x:v>92</x:v>
       </x:c>
       <x:c r="M3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="N3" s="0" t="s">
         <x:v>94</x:v>
       </x:c>
       <x:c r="O3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="P3" s="0" t="s">
         <x:v>166</x:v>
       </x:c>
       <x:c r="Q3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="R3" s="0" t="s">
         <x:v>98</x:v>
       </x:c>
       <x:c r="S3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="T3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="U3" s="0" t="s">
         <x:v>101</x:v>
@@ -1504,34 +1507,34 @@
         <x:v>102</x:v>
       </x:c>
       <x:c r="W3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="X3" s="0" t="s">
         <x:v>167</x:v>
       </x:c>
       <x:c r="Y3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="Z3" s="0" t="s">
         <x:v>106</x:v>
       </x:c>
       <x:c r="AA3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="AB3" s="0" t="s">
         <x:v>108</x:v>
       </x:c>
       <x:c r="AC3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="AD3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="AE3" s="0" t="s">
         <x:v>111</x:v>
       </x:c>
       <x:c r="AF3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="AG3" s="0" t="s">
         <x:v>113</x:v>
@@ -1540,34 +1543,34 @@
         <x:v>114</x:v>
       </x:c>
       <x:c r="AI3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="AJ3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="AK3" s="0" t="s">
         <x:v>117</x:v>
       </x:c>
       <x:c r="AL3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="AM3" s="0" t="s">
         <x:v>119</x:v>
       </x:c>
       <x:c r="AN3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="AO3" s="0" t="s">
         <x:v>121</x:v>
       </x:c>
       <x:c r="AP3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="AQ3" s="0" t="s">
         <x:v>123</x:v>
       </x:c>
       <x:c r="AR3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="AS3" s="0" t="s">
         <x:v>125</x:v>
@@ -1576,10 +1579,10 @@
         <x:v>126</x:v>
       </x:c>
       <x:c r="AU3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="AV3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="AW3" s="0" t="s">
         <x:v>129</x:v>
@@ -1594,10 +1597,10 @@
         <x:v>132</x:v>
       </x:c>
       <x:c r="BA3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="BB3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="BC3" s="0" t="s">
         <x:v>133</x:v>
@@ -1606,28 +1609,28 @@
         <x:v>135</x:v>
       </x:c>
       <x:c r="BE3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="BF3" s="0" t="s">
         <x:v>137</x:v>
       </x:c>
       <x:c r="BG3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="BH3" s="0" t="s">
         <x:v>139</x:v>
       </x:c>
       <x:c r="BI3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="BJ3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="BK3" s="0" t="s">
         <x:v>142</x:v>
       </x:c>
       <x:c r="BL3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="BM3" s="0" t="s">
         <x:v>144</x:v>
@@ -1636,34 +1639,34 @@
         <x:v>145</x:v>
       </x:c>
       <x:c r="BO3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="BP3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="BQ3" s="0" t="s">
         <x:v>148</x:v>
       </x:c>
       <x:c r="BR3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="BS3" s="0" t="s">
         <x:v>150</x:v>
       </x:c>
       <x:c r="BT3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="BU3" s="0" t="s">
         <x:v>152</x:v>
       </x:c>
       <x:c r="BV3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="BW3" s="0" t="s">
         <x:v>154</x:v>
       </x:c>
       <x:c r="BX3" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="BY3" s="0" t="s">
         <x:v>156</x:v>
@@ -1674,8 +1677,11 @@
       <x:c r="CA3" s="0" t="s">
         <x:v>158</x:v>
       </x:c>
+      <x:c r="CB3" s="0" t="s">
+        <x:v>159</x:v>
+      </x:c>
       <x:c r="CC3" s="0" t="s">
-        <x:v>159</x:v>
+        <x:v>160</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>